<commit_message>
Matcher - files loading
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t xml:space="preserve">G_OrderNumber</t>
   </si>
@@ -148,46 +148,49 @@
     <t xml:space="preserve">post</t>
   </si>
   <si>
+    <t xml:space="preserve">Blocsmb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.99487.42.004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoeterickx Miranda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerkweg 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boutersem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algemene geneeskunde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weygenstraat 10b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">016 480007</t>
+  </si>
+  <si>
     <t xml:space="preserve">algemene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evalien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swerts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.99487.42.004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hoeterickx Miranda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kerkweg 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boutersem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algemene geneeskunde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weygenstraat 10b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bertem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">016 480007</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -301,7 +304,7 @@
   <dimension ref="A1:AP3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,7 +341,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="30" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="40" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="4.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="4.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="43" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -556,10 +559,10 @@
         <v>19000182500</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>19948742004</v>

</xml_diff>

<commit_message>
Matcher - inami look up PdfMaker - l_bar_code by doctor edited to match one l_bar_code by mail label
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -304,7 +304,7 @@
   <dimension ref="A1:AP3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -341,7 +341,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="30" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="40" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="4.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="43" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -598,8 +598,8 @@
         <v>50</v>
       </c>
       <c r="Q3" s="0" t="str">
-        <f aca="false">3232110565&amp;A3&amp;"044"</f>
-        <v>323211056519000182500044</v>
+        <f aca="false">3232110565&amp;A3&amp;"045"</f>
+        <v>323211056519000182500045</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>51</v>

</xml_diff>